<commit_message>
Import task template API
</commit_message>
<xml_diff>
--- a/reports-api/src/reports_api/templates/task_template.xlsx
+++ b/reports-api/src/reports_api/templates/task_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\aot\EPIC-FLOW\reports-api\src\reports_api\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\reports-api\src\reports_api\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641D4189-1589-4B7C-ACA8-8373A3BB97E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0924B8B9-5C02-4C16-97BD-B42DB6F67570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{564F13A6-1F2F-4F4D-B303-A05BEE72DCC1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{564F13A6-1F2F-4F4D-B303-A05BEE72DCC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,23 +34,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
-  <si>
-    <t>Title</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Tips</t>
   </si>
   <si>
-    <t>StartAt</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>NumberOfDays</t>
-  </si>
-  <si>
     <t>Task 1</t>
   </si>
   <si>
@@ -67,6 +58,21 @@
   </si>
   <si>
     <t>Steps to complete</t>
+  </si>
+  <si>
+    <t>Start Plus</t>
+  </si>
+  <si>
+    <t>Task "Title"</t>
+  </si>
+  <si>
+    <t>Length (Days)</t>
+  </si>
+  <si>
+    <t>Responsibility</t>
+  </si>
+  <si>
+    <t>EAO</t>
   </si>
 </sst>
 </file>
@@ -435,123 +441,143 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912644E0-EB17-48E0-BDA4-90794DA7A383}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
+      <c r="F2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
+      <c r="F3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
+      <c r="F4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>15</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
-        <v>10</v>
+      <c r="F5" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>20</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
-        <v>10</v>
+      <c r="F6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E7:E51">
+  <conditionalFormatting sqref="F7:F51">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Import Task template events (#899)
* bugs (#894)

* Import task template API
</commit_message>
<xml_diff>
--- a/reports-api/src/reports_api/templates/task_template.xlsx
+++ b/reports-api/src/reports_api/templates/task_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\aot\EPIC-FLOW\reports-api\src\reports_api\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\reports-api\src\reports_api\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641D4189-1589-4B7C-ACA8-8373A3BB97E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0924B8B9-5C02-4C16-97BD-B42DB6F67570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{564F13A6-1F2F-4F4D-B303-A05BEE72DCC1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{564F13A6-1F2F-4F4D-B303-A05BEE72DCC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,23 +34,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
-  <si>
-    <t>Title</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Tips</t>
   </si>
   <si>
-    <t>StartAt</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>NumberOfDays</t>
-  </si>
-  <si>
     <t>Task 1</t>
   </si>
   <si>
@@ -67,6 +58,21 @@
   </si>
   <si>
     <t>Steps to complete</t>
+  </si>
+  <si>
+    <t>Start Plus</t>
+  </si>
+  <si>
+    <t>Task "Title"</t>
+  </si>
+  <si>
+    <t>Length (Days)</t>
+  </si>
+  <si>
+    <t>Responsibility</t>
+  </si>
+  <si>
+    <t>EAO</t>
   </si>
 </sst>
 </file>
@@ -435,123 +441,143 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912644E0-EB17-48E0-BDA4-90794DA7A383}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
+      <c r="F2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
+      <c r="F3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
+      <c r="F4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>15</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
-        <v>10</v>
+      <c r="F5" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>20</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
-        <v>10</v>
+      <c r="F6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E7:E51">
+  <conditionalFormatting sqref="F7:F51">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>